<commit_message>
Updated mother config to taxonomy and multiple method profiles
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/Collection_methods.xlsx
+++ b/utils/config/ReferenceLists/Collection_methods.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/jeremy_krogh_gov_bc_ca/Documents/Projects/2023/EMStoSamples/CanadaTestConfiguration/ReferenceLists/BuildItUp/AsBuiltTraining/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{0A42B53C-EDFF-453B-9F6D-C5FF344CCB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E38B0F2B-68AE-411A-8290-ADFF4D4A3DFA}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{0A42B53C-EDFF-453B-9F6D-C5FF344CCB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AE78EE0-3325-4C0F-A3E0-FB7B9E4FE47D}"/>
   <bookViews>
-    <workbookView xWindow="14775" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{FFDCD9FB-F689-4092-9462-5275F6FA98A0}"/>
+    <workbookView xWindow="-28920" yWindow="-3030" windowWidth="29040" windowHeight="15840" xr2:uid="{FFDCD9FB-F689-4092-9462-5275F6FA98A0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CollectionMethods" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CollectionMethods!$A$1:$D$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -932,16 +932,16 @@
       <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="56.26953125" customWidth="1"/>
+    <col min="3" max="3" width="65.7265625" customWidth="1"/>
     <col min="4" max="4" width="88" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +955,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="13">
         <v>25</v>
       </c>
@@ -973,7 +973,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
@@ -987,7 +987,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
@@ -1001,7 +1001,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="15" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="15" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>39</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="15" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>16</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="15" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>24</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>3</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="10" t="s">
         <v>69</v>
@@ -1233,7 +1233,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>52</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="10" t="s">
         <v>69</v>
@@ -1267,7 +1267,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="10" t="s">
         <v>69</v>
@@ -1283,7 +1283,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="10" t="s">
         <v>69</v>
@@ -1317,7 +1317,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>45</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>5</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>34</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>31</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>14</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>47</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>49</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>10</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>42</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>19</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>32</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>7</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="21">
         <v>29</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="15" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="21">
         <v>32</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
         <v>82</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>85</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="12">
         <v>30</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>88</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>90</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B43" s="8" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Partial update to code and ref files to new standards
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/Collection_methods.xlsx
+++ b/utils/config/ReferenceLists/Collection_methods.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{0A42B53C-EDFF-453B-9F6D-C5FF344CCB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AE78EE0-3325-4C0F-A3E0-FB7B9E4FE47D}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{0A42B53C-EDFF-453B-9F6D-C5FF344CCB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B1583F3-D898-401F-A721-6DA8BDE96ACA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3030" windowWidth="29040" windowHeight="15840" xr2:uid="{FFDCD9FB-F689-4092-9462-5275F6FA98A0}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FFDCD9FB-F689-4092-9462-5275F6FA98A0}"/>
   </bookViews>
   <sheets>
-    <sheet name="CollectionMethods" sheetId="1" r:id="rId1"/>
+    <sheet name="Collection_Methods" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CollectionMethods!$A$1:$D$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_Methods!$A$1:$D$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -606,6 +606,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>